<commit_message>
Adding features in data analysis
</commit_message>
<xml_diff>
--- a/Template_teste.xlsx
+++ b/Template_teste.xlsx
@@ -69,7 +69,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,12 +91,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +135,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,10 +149,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,7 +264,7 @@
       <c r="C6" s="2" t="n">
         <v>-62.3432</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="3"/>
@@ -392,7 +382,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Decreasing cognitive complexity of the code
</commit_message>
<xml_diff>
--- a/Template_teste.xlsx
+++ b/Template_teste.xlsx
@@ -169,10 +169,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="A3:C3 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -278,6 +278,7 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="3"/>
     </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -294,10 +295,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -363,6 +364,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -382,7 +384,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -392,7 +394,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>

</xml_diff>